<commit_message>
fixasi upload lagi, benerin file excel
</commit_message>
<xml_diff>
--- a/Format-Input-APBD-KabKota.xlsx
+++ b/Format-Input-APBD-KabKota.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dwi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\keprakdibi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,188 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Uraian</t>
   </si>
   <si>
-    <t>Pendapatan</t>
-  </si>
-  <si>
-    <t>PAD</t>
-  </si>
-  <si>
-    <t>Pajak daerah</t>
-  </si>
-  <si>
-    <t>Retribusi daerah</t>
-  </si>
-  <si>
-    <t>Hasil pengelolaan kekayaan daerah yang dipisahkan</t>
-  </si>
-  <si>
-    <t>Lain-lain PAD yang sah</t>
-  </si>
-  <si>
-    <t>Pendapatan Transfer</t>
-  </si>
-  <si>
-    <t>Transfer Pemerintah Pusat - Dana Perimbangan</t>
-  </si>
-  <si>
-    <t>Dana Bagi Hasil Pajak</t>
-  </si>
-  <si>
-    <t>Dana Bagi Hasil Bukan Pajak (SDA)</t>
-  </si>
-  <si>
-    <t>Dana alokasi umum</t>
-  </si>
-  <si>
-    <t>Dana alokasi khusus</t>
-  </si>
-  <si>
-    <t>Transfer Pemerintah Pusat - Lainnya</t>
-  </si>
-  <si>
-    <t>Dana Otonomi Khusus</t>
-  </si>
-  <si>
-    <t>Dana Penyesuaian</t>
-  </si>
-  <si>
-    <t>Transfer Pemerintah Provinsi</t>
-  </si>
-  <si>
-    <t>Pendapatan Bagi Hasil Pajak</t>
-  </si>
-  <si>
-    <t>Pendapatan Bagi Hasil Lainnya</t>
-  </si>
-  <si>
-    <t>Lain-lain Pendapatan yang sah</t>
-  </si>
-  <si>
-    <t>Pendapatan Hibah</t>
-  </si>
-  <si>
-    <t>Pendapatan Dana Darurat</t>
-  </si>
-  <si>
-    <t>Pendapatan Lainnya</t>
-  </si>
-  <si>
-    <t>Belanja</t>
-  </si>
-  <si>
-    <t>Belanja Operasi</t>
-  </si>
-  <si>
-    <t>Belanja Pegawai</t>
-  </si>
-  <si>
-    <t>Belanja Barang</t>
-  </si>
-  <si>
-    <t>Belanja Bunga</t>
-  </si>
-  <si>
-    <t>Belanja Subsidi</t>
-  </si>
-  <si>
-    <t>Belanja Hibah</t>
-  </si>
-  <si>
-    <t>Belanja Bantuan sosial</t>
-  </si>
-  <si>
-    <t>Belanja Bantuan Keuangan</t>
-  </si>
-  <si>
-    <t>Belanja Modal</t>
-  </si>
-  <si>
-    <t>Tanah</t>
-  </si>
-  <si>
-    <t>Peralatan dan Mesin</t>
-  </si>
-  <si>
-    <t>Gedung dan Bangunan</t>
-  </si>
-  <si>
-    <t>Jalan, irigasi dan jaringan</t>
-  </si>
-  <si>
-    <t>Aset tetap lainnya</t>
-  </si>
-  <si>
-    <t>Konstruksi Dalam Pengerjaan</t>
-  </si>
-  <si>
-    <t>Aset lainnya</t>
-  </si>
-  <si>
-    <t>Belanja tidak terduga</t>
-  </si>
-  <si>
-    <t>Transfer</t>
-  </si>
-  <si>
-    <t>Bagi Hasil Pajak ke Kab/Kota/Desa</t>
-  </si>
-  <si>
-    <t>Bagi Hasil Retribusi ke Kab/Kota/Desa</t>
-  </si>
-  <si>
-    <t>Bagi Hasil Lainnya ke Kab/Kota/Desa</t>
-  </si>
-  <si>
-    <t>Transfer Lainnya ke Kab/Kota/Desa</t>
-  </si>
-  <si>
-    <t>Belanja dan Transfer</t>
-  </si>
-  <si>
-    <t>Pembiayaan</t>
-  </si>
-  <si>
-    <t>Penerimaan Pembiayaan</t>
-  </si>
-  <si>
-    <t>SiLPA TA sebelumnya</t>
-  </si>
-  <si>
-    <t>Pencairan dana cadangan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hasil Penjualan Kekayaan Daerah yang Dipisahkan </t>
-  </si>
-  <si>
-    <t>Penerimaan Pinjaman Daerah dan Obligasi Daerah</t>
-  </si>
-  <si>
-    <t>Penerimaan Kembali Pemberian Pinjaman</t>
-  </si>
-  <si>
-    <t>Pengeluaran Pembiayaan</t>
-  </si>
-  <si>
-    <t>Pembentukan Dana Cadangan</t>
-  </si>
-  <si>
-    <t>Penyertaan Modal (Investasi) Daerah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pembayaran Pokok Utang </t>
-  </si>
-  <si>
-    <t>Pembayaran Kegiatan Lanjutan</t>
-  </si>
-  <si>
-    <t>Pengeluaran Perhitungan Pihak Ketiga</t>
-  </si>
-  <si>
     <t>Realisasi APBD</t>
   </si>
   <si>
@@ -219,6 +42,126 @@
   </si>
   <si>
     <t>isi disini</t>
+  </si>
+  <si>
+    <t>PENDAPATAN DAERAH</t>
+  </si>
+  <si>
+    <t>PEND. ASLI DAERAH (PAD)</t>
+  </si>
+  <si>
+    <t>- Pendapatan Pajak Daerah</t>
+  </si>
+  <si>
+    <t>- Retribusi Daerah</t>
+  </si>
+  <si>
+    <t>- Hsl PMD &amp; Hsl Pengel. Kek. Daerah yg dipisahkan</t>
+  </si>
+  <si>
+    <t>- Lain-Lain PAD yg Sah</t>
+  </si>
+  <si>
+    <t>DANA PERIMBANGAN</t>
+  </si>
+  <si>
+    <t>- Bagi hasil pajak dan bukan pajak</t>
+  </si>
+  <si>
+    <t>- Dana Alokasi Umum (DAU)</t>
+  </si>
+  <si>
+    <t>- Dana Alokasi Khusus (DAK)</t>
+  </si>
+  <si>
+    <t>- Dana Penguatan Infrastruktur Daerah</t>
+  </si>
+  <si>
+    <t>LAIN-LAIN PENDAPATAN YG SAH</t>
+  </si>
+  <si>
+    <t>- Pendapatan Hibah</t>
+  </si>
+  <si>
+    <t>- Dana bagi hsl pajak dr Prov &amp; pemda lainnya</t>
+  </si>
+  <si>
+    <t>- Dana Penyesuaian &amp; otonomi khusus</t>
+  </si>
+  <si>
+    <t>- Bantuan Keuangan dr Prov atau Pemda lain</t>
+  </si>
+  <si>
+    <t>- Sumbangan Pihak Ketiga</t>
+  </si>
+  <si>
+    <t>- Alokasi Kurang Bayar DAK</t>
+  </si>
+  <si>
+    <t>BELANJA DAERAH</t>
+  </si>
+  <si>
+    <t>BELANJA TIDAK LANGSUNG</t>
+  </si>
+  <si>
+    <t>- Belanja Pegawai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Belanja Barang </t>
+  </si>
+  <si>
+    <t>- Belanja Subsidi</t>
+  </si>
+  <si>
+    <t>- Belanja Hibah</t>
+  </si>
+  <si>
+    <t>- Belanja Bantuan Sosial</t>
+  </si>
+  <si>
+    <t>- Belanja Bagi Hsl kpd Prov/Kab/Kota &amp; Pemda</t>
+  </si>
+  <si>
+    <t>- Belanja Bantuan Keuangan kpd Prov/Kab/Kota/Desa</t>
+  </si>
+  <si>
+    <t>- Belanja Tidak Terduga</t>
+  </si>
+  <si>
+    <t>BELANJA LANGSUNG</t>
+  </si>
+  <si>
+    <t>- Belanja Barang dan Jasa</t>
+  </si>
+  <si>
+    <t>- Belanja Modal</t>
+  </si>
+  <si>
+    <t>SURPLUS/(DEFISIT)</t>
+  </si>
+  <si>
+    <t>PEMBIAYAAN</t>
+  </si>
+  <si>
+    <t>PENERIMAAN DAERAH</t>
+  </si>
+  <si>
+    <t>Penggunaan Sisa Lebih Perhitungan Anggaran (SILPA)</t>
+  </si>
+  <si>
+    <t>PENGELUARAN DAEARAH</t>
+  </si>
+  <si>
+    <t>Penyertaan Modal (Investasi) Pemerintah Daerah</t>
+  </si>
+  <si>
+    <t>Penguatan Modal Pemerintah Daerah</t>
+  </si>
+  <si>
+    <t>PEMBIAYAAN NETTO</t>
+  </si>
+  <si>
+    <t>SISA LEBIH PEMBIAYAAN ANGGARAN (SILPA)</t>
   </si>
 </sst>
 </file>
@@ -598,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -617,26 +560,26 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -644,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="11"/>
@@ -653,7 +596,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3">
         <v>123</v>
@@ -665,7 +608,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>124</v>
@@ -677,7 +620,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>125</v>
@@ -689,7 +632,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>126</v>
@@ -701,7 +644,7 @@
     </row>
     <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3">
         <v>127</v>
@@ -713,7 +656,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3">
         <v>128</v>
@@ -725,7 +668,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3">
         <v>129</v>
@@ -737,7 +680,7 @@
     </row>
     <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3">
         <v>130</v>
@@ -749,7 +692,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>131</v>
@@ -761,7 +704,7 @@
     </row>
     <row r="15" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>132</v>
@@ -773,7 +716,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
         <v>133</v>
@@ -785,7 +728,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3">
         <v>134</v>
@@ -795,9 +738,9 @@
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3">
         <v>135</v>
@@ -809,7 +752,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3">
         <v>136</v>
@@ -821,7 +764,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3">
         <v>137</v>
@@ -833,7 +776,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B21" s="3">
         <v>138</v>
@@ -845,7 +788,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3">
         <v>139</v>
@@ -857,7 +800,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3">
         <v>140</v>
@@ -869,7 +812,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B24" s="3">
         <v>141</v>
@@ -881,7 +824,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3">
         <v>142</v>
@@ -893,7 +836,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B26" s="3">
         <v>143</v>
@@ -905,7 +848,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3">
         <v>144</v>
@@ -917,7 +860,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B28" s="3">
         <v>145</v>
@@ -929,7 +872,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B29" s="3">
         <v>146</v>
@@ -941,7 +884,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B30" s="3">
         <v>147</v>
@@ -953,7 +896,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B31" s="3">
         <v>148</v>
@@ -965,7 +908,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B32" s="3">
         <v>149</v>
@@ -977,7 +920,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B33" s="3">
         <v>150</v>
@@ -989,7 +932,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B34" s="3">
         <v>151</v>
@@ -1001,7 +944,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B35" s="3">
         <v>152</v>
@@ -1013,7 +956,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3">
         <v>153</v>
@@ -1025,7 +968,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3">
         <v>154</v>
@@ -1037,7 +980,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3">
         <v>155</v>
@@ -1049,7 +992,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3">
         <v>156</v>
@@ -1061,7 +1004,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B40" s="3">
         <v>157</v>
@@ -1073,7 +1016,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B41" s="3">
         <v>158</v>
@@ -1085,7 +1028,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3">
         <v>159</v>
@@ -1097,7 +1040,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B43" s="3">
         <v>160</v>
@@ -1109,7 +1052,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3">
         <v>161</v>
@@ -1121,7 +1064,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B45" s="3">
         <v>162</v>
@@ -1133,7 +1076,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B46" s="3">
         <v>163</v>
@@ -1142,246 +1085,6 @@
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="3">
-        <v>164</v>
-      </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-    </row>
-    <row r="48" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="3">
-        <v>165</v>
-      </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-    </row>
-    <row r="49" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" s="3">
-        <v>166</v>
-      </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-    </row>
-    <row r="50" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B50" s="3">
-        <v>167</v>
-      </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-    </row>
-    <row r="51" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="3">
-        <v>168</v>
-      </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="3">
-        <v>169</v>
-      </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53" s="3">
-        <v>170</v>
-      </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="3">
-        <v>171</v>
-      </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" s="3">
-        <v>172</v>
-      </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56" s="3">
-        <v>173</v>
-      </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-    </row>
-    <row r="57" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B57" s="3">
-        <v>174</v>
-      </c>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-    </row>
-    <row r="58" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B58" s="3">
-        <v>175</v>
-      </c>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-    </row>
-    <row r="59" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B59" s="3">
-        <v>176</v>
-      </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B60" s="3">
-        <v>177</v>
-      </c>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B61" s="3">
-        <v>178</v>
-      </c>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-    </row>
-    <row r="62" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B62" s="3">
-        <v>179</v>
-      </c>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B63" s="3">
-        <v>180</v>
-      </c>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B64" s="3">
-        <v>181</v>
-      </c>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B65" s="3">
-        <v>182</v>
-      </c>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-    </row>
-    <row r="66" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B66" s="3">
-        <v>183</v>
-      </c>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>